<commit_message>
Add checkMostRecentObs() to the CalculationService
</commit_message>
<xml_diff>
--- a/patient-flags/src/main/resources/org/openmrs/module/drools/bp_rules.drl.xlsx
+++ b/patient-flags/src/main/resources/org/openmrs/module/drools/bp_rules.drl.xlsx
@@ -25,7 +25,7 @@
     <t>Import</t>
   </si>
   <si>
-    <t>org.openmrs.Patient,org.openmrs.module.drools.patientflags.FlaggedPatient</t>
+    <t>org.openmrs.Patient,org.openmrs.module.drools.patientflags.FlaggedPatient,org.openmrs.module.drools.calculation.Operator</t>
   </si>
   <si>
     <t>Variables</t>
@@ -52,16 +52,16 @@
     <t>$patient: Patient</t>
   </si>
   <si>
-    <t>calculationService.latestNumericObsGreaterOrEqual($patient, SYSTOLIC_UUID, $param)</t>
-  </si>
-  <si>
-    <t>calculationService.latestNumericObsLessThan($patient, SYSTOLIC_UUID, $param)</t>
-  </si>
-  <si>
-    <t>calculationService.latestNumericObsGreaterOrEqual($patient, DIASTOLIC_UUID, $param)</t>
-  </si>
-  <si>
-    <t>calculationService.latestNumericObsLessThan($patient, DIASTOLIC_UUID, $param)</t>
+    <t>calculationService.checkMostRecentObs($patient, SYSTOLIC_UUID, Operator.GTE, $param)</t>
+  </si>
+  <si>
+    <t>calculationService.checkMostRecentObs($patient, SYSTOLIC_UUID, Operator.LT, $param)</t>
+  </si>
+  <si>
+    <t>calculationService.checkMostRecentObs($patient, DIASTOLIC_UUID, Operator.GTE, $param)</t>
+  </si>
+  <si>
+    <t>calculationService.checkMostRecentObs($patient, DIASTOLIC_UUID, Operator.LT, $param)</t>
   </si>
   <si>
     <t>flaggedPatients.add(new FlaggedPatient($patient.getPatientId(), $param));</t>
@@ -162,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -170,17 +170,14 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -496,12 +493,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="29.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="57.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="72.7192857142857" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="17.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="34.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="29.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="57.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="72.7192857142857" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="47.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="34.29071428571429" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -541,8 +538,8 @@
       <c r="F3" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -632,14 +629,14 @@
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="3">
         <v>180</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3">
         <v>110</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="3"/>
       <c r="F10" s="1" t="s">
         <v>24</v>
       </c>
@@ -648,16 +645,16 @@
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="3">
         <v>160</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="3">
         <v>180</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="3">
         <v>100</v>
       </c>
-      <c r="E11" s="6"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="1" t="s">
         <v>26</v>
       </c>
@@ -666,12 +663,12 @@
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3">
         <v>90</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3">
         <v>50</v>
       </c>
       <c r="F12" s="1" t="s">

</xml_diff>